<commit_message>
completed desktop recommendation part
</commit_message>
<xml_diff>
--- a/Desktop.xlsx
+++ b/Desktop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Coding\Github_repo\ICS3U-SystemAssignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DF0017-79BD-4CE1-B9F7-44F6F76C64EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBA395B-B8E6-479F-AAA9-D4F0480DD0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8AFCC66D-E398-4341-A376-589EA72D524E}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Intel Core i3-10105</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>MSI GeForce RTX 3060</t>
+  </si>
+  <si>
+    <t>!</t>
   </si>
 </sst>
 </file>
@@ -446,214 +449,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89016E0-5FEA-41FF-BAE5-C089E22C92FE}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A2:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>160</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>140</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>40</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>38</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>50</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>50</v>
       </c>
-      <c r="H2">
-        <f>SUM(A2:F2)</f>
+      <c r="H3">
+        <f>SUM(A3:F3)</f>
         <v>478</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>290</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>120</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>90</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>65</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>70</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>55</v>
       </c>
-      <c r="H5">
-        <f>SUM(A5:F5)</f>
+      <c r="H6">
+        <f>SUM(A6:F6)</f>
         <v>690</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>17</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>460</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>150</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>140</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>200</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>70</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>55</v>
       </c>
-      <c r="H8">
-        <f>SUM(A8:F8)</f>
-        <v>1075</v>
+      <c r="G9">
+        <v>650</v>
+      </c>
+      <c r="H9">
+        <f>SUM(A9:G9)</f>
+        <v>1725</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>12</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>17</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>20</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>350</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>150</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>90</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>65</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>70</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>55</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <v>650</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <v>1530</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D12" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D13">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D14">
         <v>100</v>
       </c>
     </row>

</xml_diff>